<commit_message>
feat: add grid layout
</commit_message>
<xml_diff>
--- a/templates/salary_data.xlsx
+++ b/templates/salary_data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\192.168.118.5\暫存共用資料夾\to 勝光\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\salary_printer\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19ADEE6D-3BB3-4A06-AD56-46758F2C5BD6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54890AF2-C1DF-49E2-97B7-BBA6F9F46314}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="597" xr2:uid="{7BA8934C-802B-44B9-8983-90AB6839C2C5}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="597" xr2:uid="{7BA8934C-802B-44B9-8983-90AB6839C2C5}"/>
   </bookViews>
   <sheets>
     <sheet name="薪資表" sheetId="3" r:id="rId1"/>
@@ -174,7 +174,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="39">
   <si>
     <t>姓名</t>
   </si>
@@ -236,10 +236,6 @@
   </si>
   <si>
     <t>應發薪資</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>編号</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -323,6 +319,18 @@
   </si>
   <si>
     <t>獎金</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>密碼</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ABC</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>編號</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -439,7 +447,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -525,6 +533,15 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
@@ -532,7 +549,7 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -587,12 +604,30 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="177" fontId="7" fillId="4" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="7" fillId="4" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="7" fillId="4" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="8" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="177" fontId="7" fillId="4" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="7" fillId="4" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="177" fontId="7" fillId="4" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -617,23 +652,8 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="7" fillId="4" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="7" fillId="4" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="7" fillId="4" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="8" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="7" fillId="4" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1011,11 +1031,11 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:AD8"/>
+  <dimension ref="A1:AE8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J7" sqref="J7"/>
+      <selection pane="bottomLeft" activeCell="A3" sqref="A3:A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
@@ -1041,119 +1061,122 @@
     <col min="31" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30" ht="38.25" hidden="1">
+    <row r="1" spans="1:31" ht="38.25" hidden="1">
       <c r="A1" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B1" s="2"/>
       <c r="AC1" s="12"/>
     </row>
-    <row r="2" spans="1:30" ht="32.25" hidden="1">
+    <row r="2" spans="1:31" ht="32.25" hidden="1">
       <c r="A2" s="3" t="s">
         <v>4</v>
       </c>
       <c r="B2" s="3"/>
-      <c r="X2" s="28" t="s">
+      <c r="X2" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="Y2" s="29"/>
-      <c r="Z2" s="29"/>
-      <c r="AA2" s="29"/>
-      <c r="AB2" s="30"/>
+      <c r="Y2" s="19"/>
+      <c r="Z2" s="19"/>
+      <c r="AA2" s="19"/>
+      <c r="AB2" s="20"/>
       <c r="AC2" s="1"/>
     </row>
-    <row r="3" spans="1:30" ht="19.5" customHeight="1">
-      <c r="A3" s="23" t="s">
-        <v>16</v>
-      </c>
-      <c r="B3" s="21" t="s">
+    <row r="3" spans="1:31" ht="19.5" customHeight="1">
+      <c r="A3" s="29" t="s">
+        <v>38</v>
+      </c>
+      <c r="B3" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="23" t="s">
+      <c r="C3" s="29" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="23" t="s">
+      <c r="D3" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="E3" s="25" t="s">
+      <c r="E3" s="31" t="s">
         <v>15</v>
       </c>
-      <c r="F3" s="26"/>
-      <c r="G3" s="26"/>
-      <c r="H3" s="26"/>
-      <c r="I3" s="26"/>
-      <c r="J3" s="26"/>
-      <c r="K3" s="26"/>
-      <c r="L3" s="26"/>
-      <c r="M3" s="26"/>
-      <c r="N3" s="27"/>
-      <c r="O3" s="24" t="s">
+      <c r="F3" s="32"/>
+      <c r="G3" s="32"/>
+      <c r="H3" s="32"/>
+      <c r="I3" s="32"/>
+      <c r="J3" s="32"/>
+      <c r="K3" s="32"/>
+      <c r="L3" s="32"/>
+      <c r="M3" s="32"/>
+      <c r="N3" s="33"/>
+      <c r="O3" s="30" t="s">
         <v>13</v>
       </c>
-      <c r="P3" s="31" t="s">
-        <v>18</v>
-      </c>
-      <c r="Q3" s="31"/>
-      <c r="R3" s="31"/>
-      <c r="S3" s="31"/>
-      <c r="T3" s="31"/>
+      <c r="P3" s="21" t="s">
+        <v>17</v>
+      </c>
+      <c r="Q3" s="21"/>
+      <c r="R3" s="21"/>
+      <c r="S3" s="21"/>
+      <c r="T3" s="21"/>
       <c r="U3" s="14"/>
-      <c r="V3" s="24" t="s">
+      <c r="V3" s="30" t="s">
         <v>13</v>
       </c>
-      <c r="W3" s="32" t="s">
-        <v>20</v>
-      </c>
-      <c r="X3" s="18" t="s">
+      <c r="W3" s="22" t="s">
+        <v>19</v>
+      </c>
+      <c r="X3" s="23" t="s">
         <v>9</v>
       </c>
-      <c r="Y3" s="18" t="s">
+      <c r="Y3" s="23" t="s">
         <v>10</v>
       </c>
-      <c r="Z3" s="18" t="s">
+      <c r="Z3" s="23" t="s">
         <v>11</v>
       </c>
-      <c r="AA3" s="33" t="s">
-        <v>33</v>
-      </c>
-      <c r="AB3" s="18" t="s">
+      <c r="AA3" s="25" t="s">
+        <v>32</v>
+      </c>
+      <c r="AB3" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="AC3" s="18" t="s">
+      <c r="AC3" s="23" t="s">
         <v>14</v>
       </c>
-      <c r="AD3" s="20" t="s">
+      <c r="AD3" s="26" t="s">
         <v>1</v>
       </c>
+      <c r="AE3" s="34" t="s">
+        <v>36</v>
+      </c>
     </row>
-    <row r="4" spans="1:30" ht="39">
-      <c r="A4" s="23"/>
-      <c r="B4" s="22"/>
-      <c r="C4" s="23"/>
-      <c r="D4" s="23"/>
+    <row r="4" spans="1:31" ht="39">
+      <c r="A4" s="29"/>
+      <c r="B4" s="28"/>
+      <c r="C4" s="29"/>
+      <c r="D4" s="29"/>
       <c r="E4" s="4" t="s">
         <v>5</v>
       </c>
       <c r="F4" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="H4" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="I4" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="J4" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="G4" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="H4" s="4" t="s">
+      <c r="K4" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="I4" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="J4" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="K4" s="4" t="s">
-        <v>30</v>
-      </c>
       <c r="L4" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="M4" s="5" t="s">
         <v>6</v>
@@ -1161,36 +1184,37 @@
       <c r="N4" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="O4" s="24"/>
+      <c r="O4" s="30"/>
       <c r="P4" s="13" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="Q4" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="R4" s="13" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="S4" s="13" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="T4" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="U4" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="U4" s="13" t="s">
-        <v>25</v>
-      </c>
-      <c r="V4" s="24"/>
-      <c r="W4" s="32"/>
-      <c r="X4" s="19"/>
-      <c r="Y4" s="19"/>
-      <c r="Z4" s="19"/>
-      <c r="AA4" s="19"/>
-      <c r="AB4" s="19"/>
-      <c r="AC4" s="19"/>
-      <c r="AD4" s="20"/>
+      <c r="V4" s="30"/>
+      <c r="W4" s="22"/>
+      <c r="X4" s="24"/>
+      <c r="Y4" s="24"/>
+      <c r="Z4" s="24"/>
+      <c r="AA4" s="24"/>
+      <c r="AB4" s="24"/>
+      <c r="AC4" s="24"/>
+      <c r="AD4" s="26"/>
+      <c r="AE4" s="34"/>
     </row>
-    <row r="5" spans="1:30" s="10" customFormat="1" ht="19.5">
+    <row r="5" spans="1:31" s="10" customFormat="1" ht="19.5">
       <c r="A5" s="8">
         <v>1</v>
       </c>
@@ -1198,10 +1222,10 @@
         <v>2024</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E5" s="9">
         <v>60000</v>
@@ -1282,8 +1306,11 @@
         <v>103572</v>
       </c>
       <c r="AD5" s="16"/>
+      <c r="AE5" s="10" t="s">
+        <v>37</v>
+      </c>
     </row>
-    <row r="6" spans="1:30" s="10" customFormat="1" ht="19.5">
+    <row r="6" spans="1:31" s="10" customFormat="1" ht="19.5">
       <c r="A6" s="8">
         <v>2</v>
       </c>
@@ -1291,10 +1318,10 @@
         <v>2024</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E6" s="9">
         <v>50000</v>
@@ -1365,8 +1392,11 @@
         <v>60972</v>
       </c>
       <c r="AD6" s="16"/>
+      <c r="AE6" s="10" t="s">
+        <v>37</v>
+      </c>
     </row>
-    <row r="7" spans="1:30" s="15" customFormat="1" ht="19.5">
+    <row r="7" spans="1:31" s="15" customFormat="1" ht="19.5">
       <c r="A7" s="6">
         <v>1</v>
       </c>
@@ -1377,7 +1407,7 @@
         <v>12</v>
       </c>
       <c r="D7" s="8" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E7" s="7">
         <v>60000</v>
@@ -1440,8 +1470,11 @@
         <v>69972</v>
       </c>
       <c r="AD7" s="17"/>
+      <c r="AE7" s="15" t="s">
+        <v>37</v>
+      </c>
     </row>
-    <row r="8" spans="1:30" s="15" customFormat="1" ht="19.5">
+    <row r="8" spans="1:31" s="15" customFormat="1" ht="19.5">
       <c r="A8" s="6">
         <v>2</v>
       </c>
@@ -1452,7 +1485,7 @@
         <v>12</v>
       </c>
       <c r="D8" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E8" s="7">
         <v>60000</v>
@@ -1517,17 +1550,14 @@
         <v>68772</v>
       </c>
       <c r="AD8" s="17"/>
+      <c r="AE8" s="15" t="s">
+        <v>37</v>
+      </c>
     </row>
   </sheetData>
   <autoFilter ref="A4:AD7" xr:uid="{00CDA866-F8C2-41C0-9105-1A956E0BBC04}"/>
-  <mergeCells count="17">
-    <mergeCell ref="X2:AB2"/>
-    <mergeCell ref="P3:T3"/>
-    <mergeCell ref="W3:W4"/>
-    <mergeCell ref="Y3:Y4"/>
-    <mergeCell ref="Z3:Z4"/>
-    <mergeCell ref="AA3:AA4"/>
-    <mergeCell ref="AB3:AB4"/>
+  <mergeCells count="18">
+    <mergeCell ref="AE3:AE4"/>
     <mergeCell ref="AC3:AC4"/>
     <mergeCell ref="AD3:AD4"/>
     <mergeCell ref="B3:B4"/>
@@ -1538,6 +1568,13 @@
     <mergeCell ref="O3:O4"/>
     <mergeCell ref="X3:X4"/>
     <mergeCell ref="E3:N3"/>
+    <mergeCell ref="X2:AB2"/>
+    <mergeCell ref="P3:T3"/>
+    <mergeCell ref="W3:W4"/>
+    <mergeCell ref="Y3:Y4"/>
+    <mergeCell ref="Z3:Z4"/>
+    <mergeCell ref="AA3:AA4"/>
+    <mergeCell ref="AB3:AB4"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
refactor: split display program
</commit_message>
<xml_diff>
--- a/templates/salary_data.xlsx
+++ b/templates/salary_data.xlsx
@@ -8,12 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\salary_printer\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54890AF2-C1DF-49E2-97B7-BBA6F9F46314}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E151D675-8D14-4EB8-8160-B59DF0714981}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="597" xr2:uid="{7BA8934C-802B-44B9-8983-90AB6839C2C5}"/>
   </bookViews>
   <sheets>
     <sheet name="薪資表" sheetId="3" r:id="rId1"/>
+    <sheet name="人員" sheetId="4" r:id="rId2"/>
+    <sheet name="扣繳選擇方式說明" sheetId="5" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">薪資表!$A$4:$AD$7</definedName>
@@ -173,8 +175,26 @@
 </comments>
 </file>
 
+<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>tc={559D5BA3-A1B8-4C46-8FE4-887C07EECAAB}</author>
+  </authors>
+  <commentList>
+    <comment ref="A2" authorId="0" shapeId="0" xr:uid="{559D5BA3-A1B8-4C46-8FE4-887C07EECAAB}">
+      <text>
+        <t>[對話串註解]
+您的 Excel 版本可讓您讀取此對話串註解; 但若以較新的 Excel 版本開啟此檔案，將會移除對它進行的所有編輯。深入了解: https://go.microsoft.com/fwlink/?linkid=870924。
+註解:
+    薪資+獎金&gt;88500,薪資+獎金都扣繳5%</t>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="50">
   <si>
     <t>姓名</t>
   </si>
@@ -331,6 +351,50 @@
   </si>
   <si>
     <t>編號</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>職位</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>到職日</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>經理</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>工程師</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>分</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>合</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>分</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>合</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>扣繳選擇方式</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>薪資及津貼、獎金分別計算 ; 薪資(E-N)&gt;88500,查表扣繳 ;津貼、獎金(E+H+J+K+L-N)&gt;88500,扣繳5%</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">薪資+津貼+獎金(E+H+J+K+L-N)&gt;88500,薪資及獎金，合併扣繳5% </t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -549,7 +613,7 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -604,6 +668,48 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="14" fontId="7" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="7" fillId="3" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="7" fillId="4" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="7" fillId="4" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="177" fontId="7" fillId="4" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -620,40 +726,7 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="7" fillId="4" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="7" fillId="4" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="7" fillId="4" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1026,6 +1099,14 @@
 </ThreadedComments>
 </file>
 
+<file path=xl/threadedComments/threadedComment2.xml><?xml version="1.0" encoding="utf-8"?>
+<ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <threadedComment ref="A2" dT="2024-09-09T10:27:16.45" personId="{D4E56133-11F8-4BEA-ABB1-D5C985E4986C}" id="{559D5BA3-A1B8-4C46-8FE4-887C07EECAAB}">
+    <text>薪資+獎金&gt;88500,薪資+獎金都扣繳5%</text>
+  </threadedComment>
+</ThreadedComments>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00CDA866-F8C2-41C0-9105-1A956E0BBC04}">
   <sheetPr>
@@ -1073,87 +1154,87 @@
         <v>4</v>
       </c>
       <c r="B2" s="3"/>
-      <c r="X2" s="18" t="s">
+      <c r="X2" s="32" t="s">
         <v>8</v>
       </c>
-      <c r="Y2" s="19"/>
-      <c r="Z2" s="19"/>
-      <c r="AA2" s="19"/>
-      <c r="AB2" s="20"/>
+      <c r="Y2" s="33"/>
+      <c r="Z2" s="33"/>
+      <c r="AA2" s="33"/>
+      <c r="AB2" s="34"/>
       <c r="AC2" s="1"/>
     </row>
     <row r="3" spans="1:31" ht="19.5" customHeight="1">
-      <c r="A3" s="29" t="s">
+      <c r="A3" s="27" t="s">
         <v>38</v>
       </c>
-      <c r="B3" s="27" t="s">
+      <c r="B3" s="25" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="29" t="s">
+      <c r="C3" s="27" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="29" t="s">
+      <c r="D3" s="27" t="s">
         <v>0</v>
       </c>
-      <c r="E3" s="31" t="s">
+      <c r="E3" s="29" t="s">
         <v>15</v>
       </c>
-      <c r="F3" s="32"/>
-      <c r="G3" s="32"/>
-      <c r="H3" s="32"/>
-      <c r="I3" s="32"/>
-      <c r="J3" s="32"/>
-      <c r="K3" s="32"/>
-      <c r="L3" s="32"/>
-      <c r="M3" s="32"/>
-      <c r="N3" s="33"/>
-      <c r="O3" s="30" t="s">
+      <c r="F3" s="30"/>
+      <c r="G3" s="30"/>
+      <c r="H3" s="30"/>
+      <c r="I3" s="30"/>
+      <c r="J3" s="30"/>
+      <c r="K3" s="30"/>
+      <c r="L3" s="30"/>
+      <c r="M3" s="30"/>
+      <c r="N3" s="31"/>
+      <c r="O3" s="28" t="s">
         <v>13</v>
       </c>
-      <c r="P3" s="21" t="s">
+      <c r="P3" s="35" t="s">
         <v>17</v>
       </c>
-      <c r="Q3" s="21"/>
-      <c r="R3" s="21"/>
-      <c r="S3" s="21"/>
-      <c r="T3" s="21"/>
+      <c r="Q3" s="35"/>
+      <c r="R3" s="35"/>
+      <c r="S3" s="35"/>
+      <c r="T3" s="35"/>
       <c r="U3" s="14"/>
-      <c r="V3" s="30" t="s">
+      <c r="V3" s="28" t="s">
         <v>13</v>
       </c>
-      <c r="W3" s="22" t="s">
+      <c r="W3" s="36" t="s">
         <v>19</v>
       </c>
-      <c r="X3" s="23" t="s">
+      <c r="X3" s="22" t="s">
         <v>9</v>
       </c>
-      <c r="Y3" s="23" t="s">
+      <c r="Y3" s="22" t="s">
         <v>10</v>
       </c>
-      <c r="Z3" s="23" t="s">
+      <c r="Z3" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="AA3" s="25" t="s">
+      <c r="AA3" s="37" t="s">
         <v>32</v>
       </c>
-      <c r="AB3" s="23" t="s">
+      <c r="AB3" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="AC3" s="23" t="s">
+      <c r="AC3" s="22" t="s">
         <v>14</v>
       </c>
-      <c r="AD3" s="26" t="s">
+      <c r="AD3" s="24" t="s">
         <v>1</v>
       </c>
-      <c r="AE3" s="34" t="s">
+      <c r="AE3" s="21" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="4" spans="1:31" ht="39">
-      <c r="A4" s="29"/>
-      <c r="B4" s="28"/>
-      <c r="C4" s="29"/>
-      <c r="D4" s="29"/>
+      <c r="A4" s="27"/>
+      <c r="B4" s="26"/>
+      <c r="C4" s="27"/>
+      <c r="D4" s="27"/>
       <c r="E4" s="4" t="s">
         <v>5</v>
       </c>
@@ -1184,7 +1265,7 @@
       <c r="N4" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="O4" s="30"/>
+      <c r="O4" s="28"/>
       <c r="P4" s="13" t="s">
         <v>21</v>
       </c>
@@ -1203,16 +1284,16 @@
       <c r="U4" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="V4" s="30"/>
-      <c r="W4" s="22"/>
-      <c r="X4" s="24"/>
-      <c r="Y4" s="24"/>
-      <c r="Z4" s="24"/>
-      <c r="AA4" s="24"/>
-      <c r="AB4" s="24"/>
-      <c r="AC4" s="24"/>
-      <c r="AD4" s="26"/>
-      <c r="AE4" s="34"/>
+      <c r="V4" s="28"/>
+      <c r="W4" s="36"/>
+      <c r="X4" s="23"/>
+      <c r="Y4" s="23"/>
+      <c r="Z4" s="23"/>
+      <c r="AA4" s="23"/>
+      <c r="AB4" s="23"/>
+      <c r="AC4" s="23"/>
+      <c r="AD4" s="24"/>
+      <c r="AE4" s="21"/>
     </row>
     <row r="5" spans="1:31" s="10" customFormat="1" ht="19.5">
       <c r="A5" s="8">
@@ -1557,6 +1638,13 @@
   </sheetData>
   <autoFilter ref="A4:AD7" xr:uid="{00CDA866-F8C2-41C0-9105-1A956E0BBC04}"/>
   <mergeCells count="18">
+    <mergeCell ref="X2:AB2"/>
+    <mergeCell ref="P3:T3"/>
+    <mergeCell ref="W3:W4"/>
+    <mergeCell ref="Y3:Y4"/>
+    <mergeCell ref="Z3:Z4"/>
+    <mergeCell ref="AA3:AA4"/>
+    <mergeCell ref="AB3:AB4"/>
     <mergeCell ref="AE3:AE4"/>
     <mergeCell ref="AC3:AC4"/>
     <mergeCell ref="AD3:AD4"/>
@@ -1568,17 +1656,104 @@
     <mergeCell ref="O3:O4"/>
     <mergeCell ref="X3:X4"/>
     <mergeCell ref="E3:N3"/>
-    <mergeCell ref="X2:AB2"/>
-    <mergeCell ref="P3:T3"/>
-    <mergeCell ref="W3:W4"/>
-    <mergeCell ref="Y3:Y4"/>
-    <mergeCell ref="Z3:Z4"/>
-    <mergeCell ref="AA3:AA4"/>
-    <mergeCell ref="AB3:AB4"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="50" fitToHeight="0" orientation="landscape" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C2EEE669-DB24-4AAE-9B35-1B3B78BEDD6D}">
+  <dimension ref="A1:D3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="16.5"/>
+  <cols>
+    <col min="3" max="3" width="11.875" style="20" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.625" style="20" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="39">
+      <c r="A1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="C1" s="18" t="s">
+        <v>40</v>
+      </c>
+      <c r="D1" s="18" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="19.5">
+      <c r="A2" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="C2" s="19">
+        <v>45292</v>
+      </c>
+      <c r="D2" s="19" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="19.5">
+      <c r="A3" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="C3" s="19">
+        <v>45352</v>
+      </c>
+      <c r="D3" s="19" t="s">
+        <v>46</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ECFBE83C-D93B-48E2-B8D8-726005735CCE}">
+  <dimension ref="A3:B4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="16.5"/>
+  <cols>
+    <col min="2" max="2" width="63.375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="1:2">
+      <c r="A3" t="s">
+        <v>43</v>
+      </c>
+      <c r="B3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" t="s">
+        <v>44</v>
+      </c>
+      <c r="B4" t="s">
+        <v>49</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
chore: add mapping config
</commit_message>
<xml_diff>
--- a/templates/salary_data.xlsx
+++ b/templates/salary_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\salary_printer\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECA6810D-7AB8-4E21-8A04-CA3CD62B92BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36E5C769-48C5-48CD-AB38-E6442ED91498}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28845" yWindow="0" windowWidth="14610" windowHeight="15705" tabRatio="597" xr2:uid="{7BA8934C-802B-44B9-8983-90AB6839C2C5}"/>
+    <workbookView xWindow="28695" yWindow="0" windowWidth="14610" windowHeight="15705" tabRatio="597" xr2:uid="{7BA8934C-802B-44B9-8983-90AB6839C2C5}"/>
   </bookViews>
   <sheets>
     <sheet name="薪資表" sheetId="3" r:id="rId1"/>
@@ -1122,9 +1122,12 @@
   </sheetPr>
   <dimension ref="A1:AH8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A3" sqref="A3:A4"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <pane xSplit="4" ySplit="2" topLeftCell="E5" activePane="bottomRight" state="frozen"/>
+      <selection activeCell="A3" sqref="A3"/>
+      <selection pane="topRight" activeCell="E3" sqref="E3"/>
+      <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
+      <selection pane="bottomRight" activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
@@ -1408,7 +1411,7 @@
         <v>9931</v>
       </c>
       <c r="AF5" s="9">
-        <f t="shared" ref="AF5" si="1">Y5+AE5</f>
+        <f>Y5+AE5</f>
         <v>101572</v>
       </c>
       <c r="AG5" s="37"/>
@@ -1455,7 +1458,7 @@
       <c r="N6" s="9"/>
       <c r="O6" s="9"/>
       <c r="P6" s="9">
-        <f t="shared" ref="P6:P8" si="2">E6+F6+H6+J6+K6+L6-N6+O6</f>
+        <f t="shared" ref="P6:P8" si="1">E6+F6+H6+J6+K6+L6-N6+O6</f>
         <v>55500</v>
       </c>
       <c r="Q6" s="9">
@@ -1472,11 +1475,11 @@
       <c r="V6" s="9"/>
       <c r="W6" s="9"/>
       <c r="X6" s="9">
-        <f t="shared" ref="X6" si="3">SUM(Q6:W6)</f>
+        <f t="shared" ref="X6" si="2">SUM(Q6:W6)</f>
         <v>4959</v>
       </c>
       <c r="Y6" s="9">
-        <f t="shared" ref="Y6" si="4">P6-X6</f>
+        <f t="shared" ref="Y6" si="3">P6-X6</f>
         <v>50541</v>
       </c>
       <c r="Z6" s="9">
@@ -1493,11 +1496,11 @@
         <v>500</v>
       </c>
       <c r="AE6" s="9">
-        <f t="shared" ref="AE6:AE8" si="5">SUM(Z6:AC6)</f>
+        <f t="shared" ref="AE6:AE8" si="4">SUM(Z6:AC6)</f>
         <v>9931</v>
       </c>
       <c r="AF6" s="9">
-        <f t="shared" ref="AF6" si="6">Y6+AE6</f>
+        <f t="shared" ref="AF6" si="5">Y6+AE6</f>
         <v>60472</v>
       </c>
       <c r="AG6" s="37"/>
@@ -1534,7 +1537,7 @@
       <c r="N7" s="7"/>
       <c r="O7" s="7"/>
       <c r="P7" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>62000</v>
       </c>
       <c r="Q7" s="7">
@@ -1555,11 +1558,11 @@
       <c r="V7" s="7"/>
       <c r="W7" s="7"/>
       <c r="X7" s="7">
-        <f t="shared" ref="X7" si="7">SUM(Q7:W7)</f>
+        <f t="shared" ref="X7" si="6">SUM(Q7:W7)</f>
         <v>1959</v>
       </c>
       <c r="Y7" s="7">
-        <f t="shared" ref="Y7" si="8">P7-X7</f>
+        <f t="shared" ref="Y7" si="7">P7-X7</f>
         <v>60041</v>
       </c>
       <c r="Z7" s="7">
@@ -1578,7 +1581,7 @@
         <v>9931</v>
       </c>
       <c r="AF7" s="7">
-        <f t="shared" ref="AF7" si="9">Y7+AE7</f>
+        <f t="shared" ref="AF7" si="8">Y7+AE7</f>
         <v>69972</v>
       </c>
       <c r="AG7" s="39"/>
@@ -1617,7 +1620,7 @@
       <c r="N8" s="7"/>
       <c r="O8" s="7"/>
       <c r="P8" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>61000</v>
       </c>
       <c r="Q8" s="7">
@@ -1638,11 +1641,11 @@
       <c r="V8" s="7"/>
       <c r="W8" s="7"/>
       <c r="X8" s="7">
-        <f t="shared" ref="X8" si="10">SUM(Q8:W8)</f>
+        <f t="shared" ref="X8" si="9">SUM(Q8:W8)</f>
         <v>2159</v>
       </c>
       <c r="Y8" s="7">
-        <f t="shared" ref="Y8" si="11">P8-X8</f>
+        <f t="shared" ref="Y8" si="10">P8-X8</f>
         <v>58841</v>
       </c>
       <c r="Z8" s="7">
@@ -1657,11 +1660,11 @@
       <c r="AC8" s="7"/>
       <c r="AD8" s="7"/>
       <c r="AE8" s="9">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>9931</v>
       </c>
       <c r="AF8" s="7">
-        <f t="shared" ref="AF8" si="12">Y8+AE8</f>
+        <f t="shared" ref="AF8" si="11">Y8+AE8</f>
         <v>68772</v>
       </c>
       <c r="AG8" s="39"/>

</xml_diff>

<commit_message>
fix: break line issue
</commit_message>
<xml_diff>
--- a/templates/salary_data.xlsx
+++ b/templates/salary_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\salary_printer\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36E5C769-48C5-48CD-AB38-E6442ED91498}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{410A9D10-8847-44C3-A7FF-ED272885C840}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28695" yWindow="0" windowWidth="14610" windowHeight="15705" tabRatio="597" xr2:uid="{7BA8934C-802B-44B9-8983-90AB6839C2C5}"/>
   </bookViews>
@@ -194,7 +194,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="53">
   <si>
     <t>姓名</t>
   </si>
@@ -403,6 +403,13 @@
   </si>
   <si>
     <t>其他</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ABVKXJLJKLJS
+KJHL:JKJ:L
+kjklj;l
+許工蓋</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -612,7 +619,7 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -735,6 +742,9 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1123,11 +1133,11 @@
   <dimension ref="A1:AH8"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <pane xSplit="4" ySplit="2" topLeftCell="E5" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="2" topLeftCell="AD5" activePane="bottomRight" state="frozen"/>
       <selection activeCell="A3" sqref="A3"/>
       <selection pane="topRight" activeCell="E3" sqref="E3"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="E5" sqref="E5"/>
+      <selection pane="bottomRight" activeCell="A8" sqref="A8:XFD8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
@@ -1319,7 +1329,7 @@
       <c r="AG4" s="26"/>
       <c r="AH4" s="36"/>
     </row>
-    <row r="5" spans="1:34" s="10" customFormat="1" ht="19.5">
+    <row r="5" spans="1:34" s="10" customFormat="1" ht="78">
       <c r="A5" s="8">
         <v>1</v>
       </c>
@@ -1414,7 +1424,9 @@
         <f>Y5+AE5</f>
         <v>101572</v>
       </c>
-      <c r="AG5" s="37"/>
+      <c r="AG5" s="41" t="s">
+        <v>52</v>
+      </c>
       <c r="AH5" s="38" t="s">
         <v>37</v>
       </c>
@@ -1706,7 +1718,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C2EEE669-DB24-4AAE-9B35-1B3B78BEDD6D}">
   <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
   <cols>

</xml_diff>

<commit_message>
fix: some bugs and ignore some item not calculate
</commit_message>
<xml_diff>
--- a/templates/salary_data.xlsx
+++ b/templates/salary_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\salary_printer\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{410A9D10-8847-44C3-A7FF-ED272885C840}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1471514F-959F-47DB-BBFA-BDDD39F7D8E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28695" yWindow="0" windowWidth="14610" windowHeight="15705" tabRatio="597" xr2:uid="{7BA8934C-802B-44B9-8983-90AB6839C2C5}"/>
   </bookViews>
@@ -1133,11 +1133,11 @@
   <dimension ref="A1:AH8"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <pane xSplit="4" ySplit="2" topLeftCell="AD5" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="2" topLeftCell="R5" activePane="bottomRight" state="frozen"/>
       <selection activeCell="A3" sqref="A3"/>
       <selection pane="topRight" activeCell="E3" sqref="E3"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="A8" sqref="A8:XFD8"/>
+      <selection pane="bottomRight" activeCell="S6" sqref="S6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
@@ -1383,7 +1383,7 @@
         <v>859</v>
       </c>
       <c r="S5" s="9">
-        <v>0</v>
+        <v>300</v>
       </c>
       <c r="T5" s="9">
         <v>1000</v>
@@ -1399,11 +1399,11 @@
       </c>
       <c r="X5" s="9">
         <f>SUM(Q5:W5)</f>
-        <v>5159</v>
+        <v>5459</v>
       </c>
       <c r="Y5" s="9">
         <f t="shared" ref="Y5" si="0">P5-X5</f>
-        <v>91641</v>
+        <v>91341</v>
       </c>
       <c r="Z5" s="9">
         <v>3926</v>
@@ -1422,7 +1422,7 @@
       </c>
       <c r="AF5" s="9">
         <f>Y5+AE5</f>
-        <v>101572</v>
+        <v>101272</v>
       </c>
       <c r="AG5" s="41" t="s">
         <v>52</v>

</xml_diff>